<commit_message>
pdf referensi, penambahan interpretasi
</commit_message>
<xml_diff>
--- a/data_migrasi.xlsx
+++ b/data_migrasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fezaa\My Drive\00. Drive PC\1.STIS\6. Semester 6\Visualisasi Data dan Informasi [T]\UAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B52669-B8D2-467E-8649-B318847F2334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B843FA0D-9FB4-4DA6-A1AD-6F29ECADFB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="laki" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="total" sheetId="3" r:id="rId3"/>
     <sheet name="tabel6" sheetId="4" r:id="rId4"/>
     <sheet name="tabel7" sheetId="5" r:id="rId5"/>
-    <sheet name="tabel12.3" sheetId="6" r:id="rId6"/>
-    <sheet name="tabel11.3" sheetId="7" r:id="rId7"/>
+    <sheet name="tabel11.3" sheetId="7" r:id="rId6"/>
+    <sheet name="tabel12.3" sheetId="6" r:id="rId7"/>
     <sheet name="tabel14" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1199,12 +1199,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1228,6 +1222,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9098,8 +9098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6F87BF-3FF3-49D8-8B51-2C34A5B63BCD}">
   <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13096,7 +13096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF9C223-2321-43DA-9F51-CB11EB529CAE}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -13112,22 +13112,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="18" t="s">
         <v>277</v>
       </c>
@@ -13941,6 +13941,297 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D6ACD1-B470-4D1B-BC34-F2C61A7FB7A1}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="17">
+        <v>243822</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1108</v>
+      </c>
+      <c r="D3" s="17">
+        <v>22</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="17">
+        <v>231910</v>
+      </c>
+      <c r="C4" s="17">
+        <v>15614</v>
+      </c>
+      <c r="D4" s="17">
+        <v>132</v>
+      </c>
+      <c r="E4" s="17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="17">
+        <v>390711</v>
+      </c>
+      <c r="C5" s="17">
+        <v>208505</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1924</v>
+      </c>
+      <c r="E5" s="17">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="17">
+        <v>238167</v>
+      </c>
+      <c r="C6" s="17">
+        <v>594075</v>
+      </c>
+      <c r="D6" s="17">
+        <v>6194</v>
+      </c>
+      <c r="E6" s="17">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B7" s="17">
+        <v>77518</v>
+      </c>
+      <c r="C7" s="17">
+        <v>614594</v>
+      </c>
+      <c r="D7" s="17">
+        <v>11075</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" s="17">
+        <v>30053</v>
+      </c>
+      <c r="C8" s="17">
+        <v>463968</v>
+      </c>
+      <c r="D8" s="17">
+        <v>11205</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" s="17">
+        <v>14001</v>
+      </c>
+      <c r="C9" s="17">
+        <v>336422</v>
+      </c>
+      <c r="D9" s="17">
+        <v>9072</v>
+      </c>
+      <c r="E9" s="17">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="17">
+        <v>7487</v>
+      </c>
+      <c r="C10" s="17">
+        <v>235213</v>
+      </c>
+      <c r="D10" s="17">
+        <v>7761</v>
+      </c>
+      <c r="E10" s="17">
+        <v>3572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="17">
+        <v>5032</v>
+      </c>
+      <c r="C11" s="17">
+        <v>151295</v>
+      </c>
+      <c r="D11" s="17">
+        <v>5212</v>
+      </c>
+      <c r="E11" s="17">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" s="17">
+        <v>2697</v>
+      </c>
+      <c r="C12" s="17">
+        <v>87679</v>
+      </c>
+      <c r="D12" s="17">
+        <v>5896</v>
+      </c>
+      <c r="E12" s="17">
+        <v>15219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1592</v>
+      </c>
+      <c r="C13" s="17">
+        <v>48366</v>
+      </c>
+      <c r="D13" s="17">
+        <v>2510</v>
+      </c>
+      <c r="E13" s="17">
+        <v>15803</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" s="17">
+        <v>623</v>
+      </c>
+      <c r="C14" s="17">
+        <v>25082</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1158</v>
+      </c>
+      <c r="E14" s="17">
+        <v>14237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15" s="17">
+        <v>382</v>
+      </c>
+      <c r="C15" s="17">
+        <v>12281</v>
+      </c>
+      <c r="D15" s="17">
+        <v>437</v>
+      </c>
+      <c r="E15" s="17">
+        <v>8963</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" s="17">
+        <v>241</v>
+      </c>
+      <c r="C16" s="17">
+        <v>7359</v>
+      </c>
+      <c r="D16" s="17">
+        <v>315</v>
+      </c>
+      <c r="E16" s="17">
+        <v>10918</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3ACA08-FC6A-4D01-AE79-208EFA421D08}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -14982,302 +15273,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D6ACD1-B470-4D1B-BC34-F2C61A7FB7A1}">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="14"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>292</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="B3" s="17">
-        <v>243822</v>
-      </c>
-      <c r="C3" s="17">
-        <v>1108</v>
-      </c>
-      <c r="D3" s="17">
-        <v>22</v>
-      </c>
-      <c r="E3" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="17">
-        <v>231910</v>
-      </c>
-      <c r="C4" s="17">
-        <v>15614</v>
-      </c>
-      <c r="D4" s="17">
-        <v>132</v>
-      </c>
-      <c r="E4" s="17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>299</v>
-      </c>
-      <c r="B5" s="17">
-        <v>390711</v>
-      </c>
-      <c r="C5" s="17">
-        <v>208505</v>
-      </c>
-      <c r="D5" s="17">
-        <v>1924</v>
-      </c>
-      <c r="E5" s="17">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>300</v>
-      </c>
-      <c r="B6" s="17">
-        <v>238167</v>
-      </c>
-      <c r="C6" s="17">
-        <v>594075</v>
-      </c>
-      <c r="D6" s="17">
-        <v>6194</v>
-      </c>
-      <c r="E6" s="17">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="B7" s="17">
-        <v>77518</v>
-      </c>
-      <c r="C7" s="17">
-        <v>614594</v>
-      </c>
-      <c r="D7" s="17">
-        <v>11075</v>
-      </c>
-      <c r="E7" s="17">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="B8" s="17">
-        <v>30053</v>
-      </c>
-      <c r="C8" s="17">
-        <v>463968</v>
-      </c>
-      <c r="D8" s="17">
-        <v>11205</v>
-      </c>
-      <c r="E8" s="17">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="B9" s="17">
-        <v>14001</v>
-      </c>
-      <c r="C9" s="17">
-        <v>336422</v>
-      </c>
-      <c r="D9" s="17">
-        <v>9072</v>
-      </c>
-      <c r="E9" s="17">
-        <v>2953</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="B10" s="17">
-        <v>7487</v>
-      </c>
-      <c r="C10" s="17">
-        <v>235213</v>
-      </c>
-      <c r="D10" s="17">
-        <v>7761</v>
-      </c>
-      <c r="E10" s="17">
-        <v>3572</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11" s="17">
-        <v>5032</v>
-      </c>
-      <c r="C11" s="17">
-        <v>151295</v>
-      </c>
-      <c r="D11" s="17">
-        <v>5212</v>
-      </c>
-      <c r="E11" s="17">
-        <v>4494</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" s="17">
-        <v>2697</v>
-      </c>
-      <c r="C12" s="17">
-        <v>87679</v>
-      </c>
-      <c r="D12" s="17">
-        <v>5896</v>
-      </c>
-      <c r="E12" s="17">
-        <v>15219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>307</v>
-      </c>
-      <c r="B13" s="17">
-        <v>1592</v>
-      </c>
-      <c r="C13" s="17">
-        <v>48366</v>
-      </c>
-      <c r="D13" s="17">
-        <v>2510</v>
-      </c>
-      <c r="E13" s="17">
-        <v>15803</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="B14" s="17">
-        <v>623</v>
-      </c>
-      <c r="C14" s="17">
-        <v>25082</v>
-      </c>
-      <c r="D14" s="17">
-        <v>1158</v>
-      </c>
-      <c r="E14" s="17">
-        <v>14237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="B15" s="17">
-        <v>382</v>
-      </c>
-      <c r="C15" s="17">
-        <v>12281</v>
-      </c>
-      <c r="D15" s="17">
-        <v>437</v>
-      </c>
-      <c r="E15" s="17">
-        <v>8963</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>310</v>
-      </c>
-      <c r="B16" s="17">
-        <v>241</v>
-      </c>
-      <c r="C16" s="17">
-        <v>7359</v>
-      </c>
-      <c r="D16" s="17">
-        <v>315</v>
-      </c>
-      <c r="E16" s="17">
-        <v>10918</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7787BA40-362A-4BC1-B974-1A9A266347FA}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -15291,595 +15291,595 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="28" t="s">
         <v>312</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="29" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="22">
         <v>18455</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="22">
         <v>11135</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="22">
         <v>8420</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="23">
         <v>628</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="22">
         <v>96573</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="22">
         <v>38417</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="22">
         <v>44414</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="23">
         <v>2749</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="22">
         <v>95332</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="22">
         <v>27559</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="22">
         <v>54057</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="23">
         <v>1902</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="22">
         <v>60516</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="22">
         <v>39750</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <v>27583</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="23">
         <v>3980</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="22">
         <v>30426</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <v>12310</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <v>9509</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>678</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="22">
         <v>56454</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <v>10831</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="22">
         <v>18871</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>741</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="22">
         <v>22507</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="22">
         <v>6120</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="22">
         <v>6035</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="23">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="22">
         <v>101091</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="22">
         <v>9940</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="22">
         <v>16393</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="23">
         <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="22">
         <v>16594</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="22">
         <v>7389</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="22">
         <v>5775</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="23">
         <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="22">
         <v>35141</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="22">
         <v>51975</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="22">
         <v>5733</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="23">
         <v>1349</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="22">
         <v>64918</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="22">
         <v>109245</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="22">
         <v>31831</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="23">
         <v>6462</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="22">
         <v>474481</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="22">
         <v>169241</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="22">
         <v>59882</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="23">
         <v>12865</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="22">
         <v>636890</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="22">
         <v>45805</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="22">
         <v>88615</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="23">
         <v>7214</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="22">
         <v>84033</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="22">
         <v>71790</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="22">
         <v>21074</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="23">
         <v>1987</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <v>286968</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="22">
         <v>38233</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="22">
         <v>34727</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="23">
         <v>4426</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="22">
         <v>161763</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="22">
         <v>62033</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="22">
         <v>14858</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="23">
         <v>2334</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="22">
         <v>16468</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="22">
         <v>29523</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="22">
         <v>3128</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="23">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="22">
         <v>141228</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="22">
         <v>6368</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="22">
         <v>14588</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="23">
         <v>464</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="22">
         <v>92581</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="22">
         <v>7020</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="22">
         <v>9214</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="23">
         <v>562</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="22">
         <v>39537</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="22">
         <v>5242</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="22">
         <v>11657</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="23">
         <v>2206</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="22">
         <v>20496</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="22">
         <v>9195</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="22">
         <v>25553</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="23">
         <v>15796</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="22">
         <v>28932</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="22">
         <v>14605</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="22">
         <v>13304</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="23">
         <v>2840</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="22">
         <v>37254</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="22">
         <v>36900</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="22">
         <v>24848</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="23">
         <v>4777</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="22">
         <v>12092</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="22">
         <v>8171</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="22">
         <v>5154</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="23">
         <v>728</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="22">
         <v>18103</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="22">
         <v>5384</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="22">
         <v>7255</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="23">
         <v>588</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="22">
         <v>26983</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="22">
         <v>10526</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="22">
         <v>7323</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="23">
         <v>845</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="22">
         <v>114245</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="22">
         <v>16923</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="22">
         <v>22881</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="23">
         <v>1253</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="24">
+      <c r="B29" s="22">
         <v>54658</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="22">
         <v>8240</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="22">
         <v>11432</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="23">
         <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="24">
+      <c r="B30" s="22">
         <v>11075</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="22">
         <v>2955</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="22">
         <v>6309</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="23">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="24">
+      <c r="B31" s="22">
         <v>25112</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="22">
         <v>2625</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="22">
         <v>6099</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="23">
         <v>627</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="24">
+      <c r="B32" s="22">
         <v>16375</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="22">
         <v>5347</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="22">
         <v>4761</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="23">
         <v>527</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33" s="22">
         <v>8740</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="22">
         <v>3491</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="22">
         <v>2643</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="23">
         <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="24">
+      <c r="B34" s="22">
         <v>15716</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="22">
         <v>11145</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="22">
         <v>6915</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="23">
         <v>1538</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="26">
+      <c r="B35" s="24">
         <v>12137</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="24">
         <v>18739</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="24">
         <v>944</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>1318</v>
       </c>
     </row>

</xml_diff>